<commit_message>
added new Homework03 exercises
</commit_message>
<xml_diff>
--- a/2670/Commands.xlsx
+++ b/2670/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Desktop\ObjectOrientedProgramming\2670\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D3E36E-4D39-4A40-AD53-C0BB2E193A1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BCAC80-B42D-474B-A7BC-249ACB358D16}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="4185" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{48C714EA-042F-4A75-B636-C9ACCEBC22A3}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{48C714EA-042F-4A75-B636-C9ACCEBC22A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Git" sheetId="1" r:id="rId1"/>
@@ -478,9 +478,6 @@
     <t>proper format is to have the start curly brace { on the same line as the class/method etc, and to always include curly start and end curly braces</t>
   </si>
   <si>
-    <t>.equals or ==</t>
-  </si>
-  <si>
     <t>.equals is for objects and == is for numbers</t>
   </si>
   <si>
@@ -641,6 +638,9 @@
       </rPr>
       <t xml:space="preserve"> = new Random();</t>
     </r>
+  </si>
+  <si>
+    <t>.equals() or ==</t>
   </si>
 </sst>
 </file>
@@ -1009,13 +1009,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1105,17 +1105,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36D6898-924E-45E2-9BE8-542A4D925F84}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1163,111 +1163,111 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>63</v>
       </c>
-      <c r="C8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1284,13 +1284,13 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1335,14 +1335,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>25</v>
       </c>
@@ -1385,12 +1385,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
added more git commands
</commit_message>
<xml_diff>
--- a/2670/Commands.xlsx
+++ b/2670/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Desktop\ObjectOrientedProgramming\2670\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85535259-0EA0-4EFC-AA01-6B19FB40CE17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E8D7D-C42E-4510-80AA-A2B1C38FEEF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14385" yWindow="2505" windowWidth="27000" windowHeight="14235" xr2:uid="{48C714EA-042F-4A75-B636-C9ACCEBC22A3}"/>
+    <workbookView xWindow="-14700" yWindow="1365" windowWidth="27000" windowHeight="14235" xr2:uid="{48C714EA-042F-4A75-B636-C9ACCEBC22A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Git" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>git push</t>
   </si>
@@ -689,6 +689,18 @@
   </si>
   <si>
     <t>adds files that would regularly be ignored due to the gitignore file</t>
+  </si>
+  <si>
+    <t>git commit -a</t>
+  </si>
+  <si>
+    <t>commits all modified files to local repository</t>
+  </si>
+  <si>
+    <t>git pull --recurse-submodules</t>
+  </si>
+  <si>
+    <t>pulls everything from the remote repository and submodules and places it in the local repository</t>
   </si>
 </sst>
 </file>
@@ -1051,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AEB3F1-297D-4308-AEC2-06D18460393F}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,6 +1169,22 @@
       </c>
       <c r="C12" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited commands and methodsandconstants
</commit_message>
<xml_diff>
--- a/2670/Commands.xlsx
+++ b/2670/Commands.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Desktop\ObjectOrientedProgramming\2670\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1396A0C8-EF8D-4EC5-AA20-0119F617C4B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D55AED4-0C57-4A3B-85F7-2F607C11B958}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="1575" windowWidth="21600" windowHeight="11385" xr2:uid="{48C714EA-042F-4A75-B636-C9ACCEBC22A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{48C714EA-042F-4A75-B636-C9ACCEBC22A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Git" sheetId="1" r:id="rId1"/>
-    <sheet name="Java" sheetId="4" r:id="rId2"/>
-    <sheet name="Spark" sheetId="3" r:id="rId3"/>
-    <sheet name="Ubuntu Bash" sheetId="2" r:id="rId4"/>
-    <sheet name="Unreal Engine" sheetId="5" r:id="rId5"/>
+    <sheet name="Java Statements" sheetId="4" r:id="rId2"/>
+    <sheet name="Java Methods" sheetId="7" r:id="rId3"/>
+    <sheet name="Java Best Practices" sheetId="8" r:id="rId4"/>
+    <sheet name="Spark" sheetId="3" r:id="rId5"/>
+    <sheet name="Ubuntu Bash" sheetId="2" r:id="rId6"/>
+    <sheet name="Unreal Engine" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>git push</t>
   </si>
@@ -701,6 +703,458 @@
   </si>
   <si>
     <t>commits all modified tracked files to local repository</t>
+  </si>
+  <si>
+    <t>Shift + F1</t>
+  </si>
+  <si>
+    <t>unlocks mouse from viewport when test playing</t>
+  </si>
+  <si>
+    <t>commits everything and writes a message in line without opening up text editor</t>
+  </si>
+  <si>
+    <r>
+      <t>git commit -am "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commit message here</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>shows available branches</t>
+  </si>
+  <si>
+    <t>if multiple methods need to use scanner, declare the scanner in the main and pass it through to the method as a parameter</t>
+  </si>
+  <si>
+    <r>
+      <t>System.out.printf("</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>format string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">", </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parameters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>%Wd = integer, W characters wide, right-aligned, %-Wd = integer, w characters wide, left-aligned, %Wf = real number, W characters wide, right-aligned</t>
+  </si>
+  <si>
+    <t>%d = integers, %f = real numbers, %s = strings</t>
+  </si>
+  <si>
+    <t>%.Df = real number, rounded to D digits after decimal, %W.Df = real number, W chars wide, D digits after decimal, %W.Df = real number, W wide (left-align), D after decimal</t>
+  </si>
+  <si>
+    <t>relational operators such as &lt; and == fail on objects</t>
+  </si>
+  <si>
+    <t>equals(string), equalsIgnoreCase(string), startsWith(string), endsWith(string), contains(string)</t>
+  </si>
+  <si>
+    <t>string test methods</t>
+  </si>
+  <si>
+    <t>random class methods</t>
+  </si>
+  <si>
+    <t>nextInt(), nextInt(max), nextDouble()</t>
+  </si>
+  <si>
+    <t>returns a random integer from 0 to max - 1</t>
+  </si>
+  <si>
+    <t>random.nextDouble()</t>
+  </si>
+  <si>
+    <t>returns a random real number in the range 0.0 to 1.0</t>
+  </si>
+  <si>
+    <t>random.nextInt(max) (add n to method to increase starting number from 0)</t>
+  </si>
+  <si>
+    <t>exception handling methods</t>
+  </si>
+  <si>
+    <t>try listens for exceptions, catch processes exceptions, throw generates exceptions, throws declares a method may throw an exception, finally defines code that must be executed before a method returns</t>
+  </si>
+  <si>
+    <t>file methods</t>
+  </si>
+  <si>
+    <t>canRead(), delete(), exists(), getName(), length(), renameTo()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scanner </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = new Scanner(new File("</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>filename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"));</t>
+    </r>
+  </si>
+  <si>
+    <t>to read a file, pass a file when constructing a Scanner</t>
+  </si>
+  <si>
+    <t>when writing file paths pay attention to absolute path (/) vs. relative path (no /)</t>
+  </si>
+  <si>
+    <t>Scanner tests for valid input</t>
+  </si>
+  <si>
+    <t>hasNext(), hasNextInt(), hasNextDouble()</t>
+  </si>
+  <si>
+    <t>line based scanner methods</t>
+  </si>
+  <si>
+    <t>nextLine(), hasNextLine()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PrintStream </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = new PrinterStream(new File("</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>filename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"));</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>any methods used on System.out (print, println) will work on PrintStream (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.println("Hello world"))</t>
+    </r>
+  </si>
+  <si>
+    <t>.next() methods don't consume newline characters, so using .nextLine() after one will return empty</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; ? &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expression1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; : &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expression2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>ternary operator, allows to choose between two expressions based on the value of a boolean test</t>
+  </si>
+  <si>
+    <t>many programmers discourage break and continue statements because these tatements cause the code execution to jump from one place to another</t>
+  </si>
+  <si>
+    <t>switch statements are also discouraged because its so easy to produce bugs</t>
+  </si>
+  <si>
+    <r>
+      <t>try {&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>statements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;;} catch (&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;) {&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>statements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;;}</t>
+    </r>
+  </si>
+  <si>
+    <t>try catch block format</t>
+  </si>
+  <si>
+    <t>when using boolean expressions simplify them using De Morgan's laws and negation when possible</t>
   </si>
 </sst>
 </file>
@@ -1063,19 +1517,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AEB3F1-297D-4308-AEC2-06D18460393F}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1083,7 +1537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1099,7 +1553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1107,7 +1561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1115,7 +1569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1123,7 +1577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1131,7 +1585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1147,7 +1601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1155,7 +1609,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1163,7 +1617,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -1171,7 +1625,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1179,12 +1633,28 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
       <c r="C14" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1195,19 +1665,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36D6898-924E-45E2-9BE8-542A4D925F84}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -1215,7 +1685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1223,7 +1693,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1231,7 +1701,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1239,7 +1709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1247,7 +1717,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1255,7 +1725,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1263,7 +1733,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -1271,7 +1741,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1279,7 +1749,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1287,79 +1757,70 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>68</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1369,6 +1830,198 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4640AA8-9FE1-4D5A-9B69-9229ACAD3952}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="169.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD14ED10-246C-4488-AF12-CCA2756767BD}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E83C7715-ECC3-486F-9050-790EBC0263EB}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1376,13 +2029,13 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1390,7 +2043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1398,7 +2051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1406,7 +2059,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1419,7 +2072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6F78D0-E2DF-4ABF-845A-13A7A93802EF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1427,14 +2080,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +2095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1450,7 +2103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1458,7 +2111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>25</v>
       </c>
@@ -1469,25 +2122,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E8593D-BC99-434E-9083-C07B224EF536}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added makeup exam programs
</commit_message>
<xml_diff>
--- a/2670/Commands.xlsx
+++ b/2670/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Desktop\ObjectOrientedProgramming\2670\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D55AED4-0C57-4A3B-85F7-2F607C11B958}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47547EB-90E3-49C8-8C84-BDF703AFE91D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{48C714EA-042F-4A75-B636-C9ACCEBC22A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{48C714EA-042F-4A75-B636-C9ACCEBC22A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Git" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>git push</t>
   </si>
@@ -1155,6 +1155,9 @@
   </si>
   <si>
     <t>when using boolean expressions simplify them using De Morgan's laws and negation when possible</t>
+  </si>
+  <si>
+    <t>* NOTE page 377 for File Objects methods</t>
   </si>
 </sst>
 </file>
@@ -1667,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36D6898-924E-45E2-9BE8-542A4D925F84}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1831,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4640AA8-9FE1-4D5A-9B69-9229ACAD3952}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1931,6 +1934,11 @@
         <v>68</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1940,7 +1948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD14ED10-246C-4488-AF12-CCA2756767BD}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>